<commit_message>
fix logo in generated pdf
</commit_message>
<xml_diff>
--- a/controller/exports/boardinghouses.xlsx
+++ b/controller/exports/boardinghouses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>No.</t>
   </si>
@@ -31,34 +31,28 @@
     <t>Zone</t>
   </si>
   <si>
-    <t>UEP Men's Dorm</t>
-  </si>
-  <si>
-    <t>UEP Main Campus</t>
-  </si>
-  <si>
-    <t>99400</t>
-  </si>
-  <si>
-    <t>Nemo perferendis dolij</t>
+    <t>Kantunan sa UEP</t>
+  </si>
+  <si>
+    <t>Ivan Joseph G. Arang</t>
+  </si>
+  <si>
+    <t>09385050074</t>
+  </si>
+  <si>
+    <t>Avelino Street</t>
   </si>
   <si>
     <t>Zone 3</t>
   </si>
   <si>
-    <t>UEP Women's Dorm</t>
-  </si>
-  <si>
-    <t>UEP</t>
-  </si>
-  <si>
-    <t>626</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incididunt amet et </t>
-  </si>
-  <si>
-    <t>Zone 1</t>
+    <t>House of Lanister</t>
+  </si>
+  <si>
+    <t>Melvin Dionisio</t>
+  </si>
+  <si>
+    <t>09518015683</t>
   </si>
 </sst>
 </file>
@@ -501,10 +495,10 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload blank file breaks server fixed
</commit_message>
<xml_diff>
--- a/controller/exports/boardinghouses.xlsx
+++ b/controller/exports/boardinghouses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>No.</t>
   </si>
@@ -31,136 +31,55 @@
     <t>Zone</t>
   </si>
   <si>
-    <t>IJA's Boarding House</t>
-  </si>
-  <si>
-    <t>Ivan Arang</t>
-  </si>
-  <si>
-    <t>09314343243</t>
-  </si>
-  <si>
-    <t>Veloso Blvd</t>
+    <t>IJA's Boarding house</t>
+  </si>
+  <si>
+    <t>Ivan Joseph Arang</t>
+  </si>
+  <si>
+    <t>09938837091</t>
+  </si>
+  <si>
+    <t>Avelino Street</t>
+  </si>
+  <si>
+    <t>Zone 3</t>
+  </si>
+  <si>
+    <t>Bahay ni Jhelan</t>
+  </si>
+  <si>
+    <t>Jhelan Anabo</t>
+  </si>
+  <si>
+    <t>0998083892</t>
+  </si>
+  <si>
+    <t>House of Tyrell</t>
+  </si>
+  <si>
+    <t>Melvin Dionisio</t>
+  </si>
+  <si>
+    <t>09837348720</t>
+  </si>
+  <si>
+    <t>Veloso Blvd.</t>
   </si>
   <si>
     <t>Zone 2</t>
   </si>
   <si>
-    <t>Portes bhaus</t>
-  </si>
-  <si>
-    <t>Rafael Portes</t>
-  </si>
-  <si>
-    <t>0912312323</t>
-  </si>
-  <si>
-    <t>Seaside Drv.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dela Cruz </t>
-  </si>
-  <si>
-    <t>Juan Dela Cruz</t>
-  </si>
-  <si>
-    <t>09324234234</t>
-  </si>
-  <si>
-    <t>Avelino Street</t>
-  </si>
-  <si>
-    <t>Zone 3</t>
-  </si>
-  <si>
-    <t>Juan for all boarding house</t>
-  </si>
-  <si>
-    <t>Juan Joseph</t>
-  </si>
-  <si>
-    <t>0932423432</t>
-  </si>
-  <si>
-    <t>Gino's House</t>
-  </si>
-  <si>
-    <t>Gino Castillo</t>
-  </si>
-  <si>
-    <t>093242343</t>
-  </si>
-  <si>
-    <t>Veloso Blvd.</t>
-  </si>
-  <si>
-    <t>Manalo's Rest house and Boarding house</t>
-  </si>
-  <si>
-    <t>Jose Manalo</t>
-  </si>
-  <si>
-    <t>091415272245</t>
+    <t>RPG B-House</t>
+  </si>
+  <si>
+    <t>Rafael P. Gumarao</t>
+  </si>
+  <si>
+    <t>09983748192</t>
   </si>
   <si>
     <t>Western Divide</t>
-  </si>
-  <si>
-    <t>Happy Living Boarding house</t>
-  </si>
-  <si>
-    <t>Toni Smith</t>
-  </si>
-  <si>
-    <t>9162543826</t>
-  </si>
-  <si>
-    <t>XYZ boarding house</t>
-  </si>
-  <si>
-    <t>Happy Danohog</t>
-  </si>
-  <si>
-    <t>09728628262</t>
-  </si>
-  <si>
-    <t>Balite St.</t>
-  </si>
-  <si>
-    <t>Zone 1</t>
-  </si>
-  <si>
-    <t>Raval's Boarding house</t>
-  </si>
-  <si>
-    <t>AJ Raval</t>
-  </si>
-  <si>
-    <t>0973826498</t>
-  </si>
-  <si>
-    <t>Hillside Drive</t>
-  </si>
-  <si>
-    <t>Castillo's Boarding house</t>
-  </si>
-  <si>
-    <t>Carlito Castillo</t>
-  </si>
-  <si>
-    <t>09725262829</t>
-  </si>
-  <si>
-    <t>Asinas Ave.</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Ivaan Arang</t>
-  </si>
-  <si>
-    <t>09</t>
   </si>
 </sst>
 </file>
@@ -541,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -603,7 +522,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -614,19 +533,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -634,159 +553,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>